<commit_message>
List test feature for test case
</commit_message>
<xml_diff>
--- a/docs/test/test-cases template-v1.1.xlsx
+++ b/docs/test/test-cases template-v1.1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vunguyen/Google Drive/Data/Courses/CS 300 - Fall 2018/Projects/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PA\Year 3\Software Engineering\Lab\E-commerce\E-commerce_Web_Application\docs\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0842163B-F5F8-43EB-8A83-DC4EEAB01B6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26160" windowHeight="15320" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="2" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -61,19 +62,6 @@
 2. The error message should be displayed</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>1. Allows the user to proceed and
-2. The error message is not displayed</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>TDHoang</t>
-  </si>
-  <si>
     <t>Login with blank Password</t>
   </si>
   <si>
@@ -89,9 +77,6 @@
     <t>Function 01: Login as admin</t>
   </si>
   <si>
-    <t>Function 02: Login as end user</t>
-  </si>
-  <si>
     <t>UC01</t>
   </si>
   <si>
@@ -117,27 +102,14 @@
   </si>
   <si>
     <t>UI04</t>
-  </si>
-  <si>
-    <t>HTThanh</t>
-  </si>
-  <si>
-    <t>NKHuy</t>
   </si>
   <si>
     <t>1. Authenticated
 2. A welcome message will  be displayed</t>
   </si>
   <si>
-    <t>The same ER</t>
-  </si>
-  <si>
     <t>1. Unauthenticated
 2. A wrong user-account notice will  be displayed</t>
-  </si>
-  <si>
-    <t>1. Unauthenticated
-2. No notice is shown</t>
   </si>
   <si>
     <t>Login with Special characters of User name and Password</t>
@@ -484,13 +456,127 @@
   </si>
   <si>
     <t>Function/Feature ID</t>
+  </si>
+  <si>
+    <t>Function 02: Login as customer</t>
+  </si>
+  <si>
+    <t>Function 03: Register as admin</t>
+  </si>
+  <si>
+    <t>Function 04: Register as customer</t>
+  </si>
+  <si>
+    <t>Function 05: Make purchase</t>
+  </si>
+  <si>
+    <t>Function 06: Search product</t>
+  </si>
+  <si>
+    <t>Function 07: Browse product</t>
+  </si>
+  <si>
+    <t>Function 08: View cart</t>
+  </si>
+  <si>
+    <t>Function 09: Edit products in cart</t>
+  </si>
+  <si>
+    <t>Function 10: Remove products from carts</t>
+  </si>
+  <si>
+    <t>Function 11: Add a product to cart</t>
+  </si>
+  <si>
+    <t>Function 12: Payment</t>
+  </si>
+  <si>
+    <t>Function 13: Add new product</t>
+  </si>
+  <si>
+    <t>Function 14: Edit product</t>
+  </si>
+  <si>
+    <t>Function 15: Delete product</t>
+  </si>
+  <si>
+    <t>Function 16: Edit profile as admin</t>
+  </si>
+  <si>
+    <t>Function 17: Edit profile as customer</t>
+  </si>
+  <si>
+    <t>UC03</t>
+  </si>
+  <si>
+    <t>UC04</t>
+  </si>
+  <si>
+    <t>UC05</t>
+  </si>
+  <si>
+    <t>UC06</t>
+  </si>
+  <si>
+    <t>UC08</t>
+  </si>
+  <si>
+    <t>UC09</t>
+  </si>
+  <si>
+    <t>UC10</t>
+  </si>
+  <si>
+    <t>UC11</t>
+  </si>
+  <si>
+    <t>UC7</t>
+  </si>
+  <si>
+    <t>UC12</t>
+  </si>
+  <si>
+    <t>UC13</t>
+  </si>
+  <si>
+    <t>UC14</t>
+  </si>
+  <si>
+    <t>UC15</t>
+  </si>
+  <si>
+    <t>UC16</t>
+  </si>
+  <si>
+    <t>UC17</t>
+  </si>
+  <si>
+    <t>UC18</t>
+  </si>
+  <si>
+    <t>UC19</t>
+  </si>
+  <si>
+    <t>UC20</t>
+  </si>
+  <si>
+    <t>Function 18: Forgot password as admin</t>
+  </si>
+  <si>
+    <t>Function 19: Forgot password as customer</t>
+  </si>
+  <si>
+    <t>Function 20: View shopping history</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -509,6 +595,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -563,13 +655,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -603,30 +700,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:D9" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A5:D9" totalsRowShown="0">
   <tableColumns count="4">
-    <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Feature Name"/>
-    <tableColumn id="3" name="Description"/>
-    <tableColumn id="4" name="Remark"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Feature Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J10" totalsRowShown="0" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:J31" totalsRowShown="0" dataDxfId="6">
   <tableColumns count="10">
-    <tableColumn id="1" name="Function/Feature ID"/>
-    <tableColumn id="11" name="Case ID"/>
-    <tableColumn id="2" name="Test case name"/>
-    <tableColumn id="4" name="Test step" dataDxfId="5"/>
-    <tableColumn id="5" name="Expected Result (ER)" dataDxfId="4"/>
-    <tableColumn id="6" name="Actual Result" dataDxfId="3"/>
-    <tableColumn id="7" name="Status" dataDxfId="2"/>
-    <tableColumn id="8" name="Tester" dataDxfId="1"/>
-    <tableColumn id="9" name="Tested Date" dataDxfId="0"/>
-    <tableColumn id="10" name="Remark"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Function/Feature ID"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Case ID"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test case name"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Test step" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Expected Result (ER)" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actual Result" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Status" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Tester" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Tested Date" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Remark"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -918,62 +1015,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" customWidth="1"/>
-    <col min="2" max="2" width="31.6640625" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -985,30 +1082,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
-    <col min="5" max="5" width="27.83203125" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1017,7 +1114,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1035,9 +1132,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1049,125 +1146,92 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="3">
-        <v>41429</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="3">
-        <v>41429</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="3">
-        <v>41429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="3">
-        <v>41429</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1179,94 +1243,1131 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3">
-        <v>41429</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3">
-        <v>41429</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.2">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3">
-        <v>41459</v>
-      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="9"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="9"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="9"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="9"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="9"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="9"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="9"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="4"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="9"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="9"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="9"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="4"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="9"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="9"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="9"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="4"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="9"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="9"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="9"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="4"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="9"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
+      <c r="H69" s="2"/>
+      <c r="I69" s="9"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="9"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="4"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="9"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="9"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="9"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="4"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="9"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B77" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="9"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="9"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="4"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="9"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="9"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B82" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Add test case for comment and rating
</commit_message>
<xml_diff>
--- a/docs/test/test-cases template-v1.1.xlsx
+++ b/docs/test/test-cases template-v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PA\Year 3\Software Engineering\Lab\E-commerce\E-commerce_Web_Application\docs\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB0E550-FA2A-467C-A576-5BE123BF782E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36A7C2B-5F5B-40B9-8F38-077A1A8F4BE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="90">
   <si>
     <t>ID</t>
   </si>
@@ -594,6 +594,18 @@
   </si>
   <si>
     <t>Register with registered username</t>
+  </si>
+  <si>
+    <t>UC21</t>
+  </si>
+  <si>
+    <t>Function 21: Add comment</t>
+  </si>
+  <si>
+    <t>UC22</t>
+  </si>
+  <si>
+    <t>Function 22: Add rating</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,6 +2604,82 @@
       <c r="H93" s="2"/>
       <c r="I93" s="9"/>
     </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="4"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>86</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>86</v>
+      </c>
+      <c r="B96" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="8"/>
+      <c r="J98" s="4"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>88</v>
+      </c>
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>88</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Count test case passed
</commit_message>
<xml_diff>
--- a/docs/test/test-cases template-v1.1.xlsx
+++ b/docs/test/test-cases template-v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PA\Year 3\Software Engineering\Lab\E-commerce\E-commerce_Web_Application\docs\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493FF349-CBC8-4F12-BC20-F05A05375FDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C9835A-AAB0-4C90-9C6A-0A2962DB6918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="530">
   <si>
     <t>Function/Feature ID</t>
   </si>
@@ -10316,6 +10316,15 @@
       </rPr>
       <t>" button</t>
     </r>
+  </si>
+  <si>
+    <t>Not test</t>
+  </si>
+  <si>
+    <t>UC12</t>
+  </si>
+  <si>
+    <t>Fixed</t>
   </si>
 </sst>
 </file>
@@ -10325,7 +10334,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10400,8 +10409,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10436,8 +10452,13 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -10472,13 +10493,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10571,10 +10608,29 @@
     <xf numFmtId="14" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -10950,10 +11006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J255"/>
+  <dimension ref="A1:O255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10967,10 +11023,15 @@
     <col min="8" max="8" width="21.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="4"/>
+    <col min="11" max="11" width="8.85546875" style="4"/>
+    <col min="12" max="12" width="10.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="4"/>
+    <col min="15" max="15" width="8" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -11001,8 +11062,17 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="33">
+        <f>COUNTIF($G$3:$G$255, "Good")</f>
+        <v>104</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -11015,8 +11085,22 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="L2" s="34" t="s">
+        <v>463</v>
+      </c>
+      <c r="M2" s="33">
+        <f>COUNTIF($G$3:$G$255, "Fail")</f>
+        <v>24</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>529</v>
+      </c>
+      <c r="O2" s="37">
+        <f>COUNTIF(J:J,"*"&amp;"fixed"&amp;"*")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
@@ -11044,8 +11128,17 @@
       <c r="I3" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="L3" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="M3" s="33">
+        <f>COUNTIF($G$3:$G$255, "Passable")</f>
+        <v>9</v>
+      </c>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -11073,8 +11166,17 @@
       <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="L4" s="33" t="s">
+        <v>527</v>
+      </c>
+      <c r="M4" s="33">
+        <f>COUNTIF($G$3:$G$255, "")-25</f>
+        <v>91</v>
+      </c>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -11103,7 +11205,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -11132,7 +11234,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -11161,7 +11263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -11193,7 +11295,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -11222,7 +11324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
@@ -11236,7 +11338,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>39</v>
       </c>
@@ -11265,7 +11367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>39</v>
       </c>
@@ -11294,7 +11396,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -11323,7 +11425,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
@@ -11352,7 +11454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -11381,7 +11483,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>39</v>
       </c>
@@ -16983,7 +17085,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17141,7 +17243,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>225</v>
+        <v>528</v>
       </c>
       <c r="B17" t="s">
         <v>415</v>
@@ -17152,7 +17254,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="B18" t="s">
         <v>417</v>
@@ -17163,7 +17265,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="B19" t="s">
         <v>261</v>
@@ -17174,7 +17276,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B20" t="s">
         <v>420</v>
@@ -17185,7 +17287,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="B21" t="s">
         <v>422</v>
@@ -17196,7 +17298,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B22" t="s">
         <v>424</v>
@@ -17207,7 +17309,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B23" t="s">
         <v>426</v>
@@ -17218,7 +17320,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B24" t="s">
         <v>428</v>
@@ -17229,7 +17331,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B25" t="s">
         <v>430</v>
@@ -17240,7 +17342,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="B26" t="s">
         <v>432</v>
@@ -17251,7 +17353,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="B27" t="s">
         <v>434</v>
@@ -17261,8 +17363,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>323</v>
+      <c r="A28" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="B28" t="s">
         <v>436</v>
@@ -17272,8 +17374,8 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>362</v>
+      <c r="A29" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="B29" t="s">
         <v>438</v>
@@ -17284,7 +17386,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="B30" t="s">
         <v>440</v>

</xml_diff>